<commit_message>
fix: bill doc: add bill pdf
</commit_message>
<xml_diff>
--- a/script/测试用例 冷 手算.xlsx
+++ b/script/测试用例 冷 手算.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29868" windowHeight="13500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="21600" windowHeight="10480" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="参数配置" sheetId="6" r:id="rId1"/>
@@ -1710,14 +1710,14 @@
       <selection activeCell="B21" sqref="B21:Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="15.462962962963" customWidth="1"/>
-    <col min="3" max="3" width="10.3796296296296" customWidth="1"/>
-    <col min="4" max="4" width="12.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="15.4636363636364" customWidth="1"/>
+    <col min="3" max="3" width="10.3818181818182" customWidth="1"/>
+    <col min="4" max="4" width="12.1090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:20">
+    <row r="1" ht="16.5" spans="1:20">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="S1" s="14"/>
       <c r="T1" s="14"/>
     </row>
-    <row r="2" ht="15.6" spans="1:20">
+    <row r="2" ht="16.5" spans="1:20">
       <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="S2" s="14"/>
       <c r="T2" s="14"/>
     </row>
-    <row r="3" ht="15.6" spans="1:20">
+    <row r="3" ht="16.5" spans="1:20">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -1795,7 +1795,7 @@
       <c r="S3" s="14"/>
       <c r="T3" s="14"/>
     </row>
-    <row r="4" ht="15.6" spans="1:19">
+    <row r="4" ht="16.5" spans="1:19">
       <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
@@ -1820,7 +1820,7 @@
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
     </row>
-    <row r="5" ht="15.6" spans="1:19">
+    <row r="5" ht="16.5" spans="1:19">
       <c r="A5" s="39" t="s">
         <v>7</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="R5" s="14"/>
       <c r="S5" s="14"/>
     </row>
-    <row r="6" ht="15.6" spans="1:19">
+    <row r="6" ht="16.5" spans="1:19">
       <c r="A6" s="39"/>
       <c r="B6" s="29" t="s">
         <v>10</v>
@@ -1874,7 +1874,7 @@
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
     </row>
-    <row r="7" ht="15.6" spans="1:19">
+    <row r="7" ht="16.5" spans="1:19">
       <c r="A7" s="39"/>
       <c r="B7" s="29" t="s">
         <v>13</v>
@@ -1899,7 +1899,7 @@
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
     </row>
-    <row r="8" ht="15.6" spans="1:20">
+    <row r="8" ht="16.5" spans="1:20">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="S8" s="14"/>
       <c r="T8" s="14"/>
     </row>
-    <row r="9" ht="15.6" spans="1:20">
+    <row r="9" ht="16.5" spans="1:20">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
         <v>16</v>
@@ -1951,7 +1951,7 @@
       <c r="S9" s="14"/>
       <c r="T9" s="14"/>
     </row>
-    <row r="10" ht="15.6" spans="1:20">
+    <row r="10" ht="16.5" spans="1:20">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
         <v>18</v>
@@ -1979,7 +1979,7 @@
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
     </row>
-    <row r="11" ht="15.6" spans="1:20">
+    <row r="11" ht="16.5" spans="1:20">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
         <v>20</v>
@@ -2007,7 +2007,7 @@
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
     </row>
-    <row r="12" ht="15.6" spans="1:20">
+    <row r="12" ht="16.5" spans="1:20">
       <c r="A12" s="11"/>
       <c r="B12" s="11" t="s">
         <v>22</v>
@@ -2035,7 +2035,7 @@
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
     </row>
-    <row r="13" ht="15.6" spans="1:20">
+    <row r="13" ht="16.5" spans="1:20">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
         <v>24</v>
@@ -2063,7 +2063,7 @@
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
     </row>
-    <row r="14" ht="15.6" spans="1:21">
+    <row r="14" ht="16.5" spans="1:21">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="41"/>
@@ -2086,7 +2086,7 @@
       <c r="T14" s="14"/>
       <c r="U14" s="14"/>
     </row>
-    <row r="15" ht="15.6" spans="1:21">
+    <row r="15" ht="16.5" spans="1:21">
       <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="T15" s="42"/>
       <c r="U15" s="42"/>
     </row>
-    <row r="16" ht="15.6" spans="1:21">
+    <row r="16" ht="16.5" spans="1:21">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -2140,7 +2140,7 @@
       <c r="T16" s="42"/>
       <c r="U16" s="42"/>
     </row>
-    <row r="17" ht="15.6" spans="1:21">
+    <row r="17" ht="16.5" spans="1:21">
       <c r="A17" s="11" t="s">
         <v>29</v>
       </c>
@@ -2167,7 +2167,7 @@
       <c r="T17" s="42"/>
       <c r="U17" s="42"/>
     </row>
-    <row r="18" ht="15.6" spans="1:21">
+    <row r="18" ht="16.5" spans="1:21">
       <c r="A18" s="11" t="s">
         <v>31</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="T18" s="42"/>
       <c r="U18" s="42"/>
     </row>
-    <row r="19" ht="31.2" spans="1:21">
+    <row r="19" ht="33" spans="1:21">
       <c r="A19" s="43" t="s">
         <v>33</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="T19" s="50"/>
       <c r="U19" s="50"/>
     </row>
-    <row r="20" ht="15.6" spans="1:17">
+    <row r="20" ht="16.5" spans="1:17">
       <c r="A20" s="43" t="s">
         <v>35</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="P20" s="44"/>
       <c r="Q20" s="51"/>
     </row>
-    <row r="21" ht="31.2" spans="1:17">
+    <row r="21" ht="33" spans="1:17">
       <c r="A21" s="43" t="s">
         <v>37</v>
       </c>
@@ -2267,7 +2267,7 @@
       <c r="P21" s="44"/>
       <c r="Q21" s="44"/>
     </row>
-    <row r="22" ht="15.6" spans="1:17">
+    <row r="22" ht="16.5" spans="1:17">
       <c r="A22" s="43" t="s">
         <v>39</v>
       </c>
@@ -2290,7 +2290,7 @@
       <c r="P22" s="44"/>
       <c r="Q22" s="51"/>
     </row>
-    <row r="23" ht="15.6" spans="1:17">
+    <row r="23" ht="16.5" spans="1:17">
       <c r="A23" s="43" t="s">
         <v>41</v>
       </c>
@@ -2313,7 +2313,7 @@
       <c r="P23" s="44"/>
       <c r="Q23" s="51"/>
     </row>
-    <row r="24" ht="31.2" spans="1:17">
+    <row r="24" ht="33" spans="1:17">
       <c r="A24" s="43" t="s">
         <v>43</v>
       </c>
@@ -2336,7 +2336,7 @@
       <c r="P24" s="44"/>
       <c r="Q24" s="51"/>
     </row>
-    <row r="25" ht="15.6" spans="1:17">
+    <row r="25" ht="16.5" spans="1:17">
       <c r="A25" s="45" t="s">
         <v>45</v>
       </c>
@@ -2536,30 +2536,30 @@
   <sheetPr/>
   <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="R18:S19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.6296296296296" customWidth="1"/>
-    <col min="2" max="3" width="7.37962962962963" customWidth="1"/>
-    <col min="4" max="6" width="7.75" customWidth="1"/>
-    <col min="7" max="7" width="6.25" customWidth="1"/>
+    <col min="1" max="1" width="10.6272727272727" customWidth="1"/>
+    <col min="2" max="3" width="7.38181818181818" customWidth="1"/>
+    <col min="4" max="6" width="7.75454545454545" customWidth="1"/>
+    <col min="7" max="7" width="6.25454545454545" customWidth="1"/>
     <col min="8" max="10" width="5.5" customWidth="1"/>
-    <col min="11" max="11" width="6.25" customWidth="1"/>
+    <col min="11" max="11" width="6.25454545454545" customWidth="1"/>
     <col min="12" max="14" width="5.5" customWidth="1"/>
-    <col min="15" max="15" width="6.25" customWidth="1"/>
+    <col min="15" max="15" width="6.25454545454545" customWidth="1"/>
     <col min="16" max="18" width="5.5" customWidth="1"/>
-    <col min="19" max="19" width="6.25" customWidth="1"/>
+    <col min="19" max="19" width="6.25454545454545" customWidth="1"/>
     <col min="20" max="21" width="5.5" customWidth="1"/>
-    <col min="22" max="23" width="6.25" customWidth="1"/>
+    <col min="22" max="23" width="6.25454545454545" customWidth="1"/>
     <col min="24" max="25" width="5.5" customWidth="1"/>
-    <col min="26" max="26" width="6.25" customWidth="1"/>
+    <col min="26" max="26" width="6.25454545454545" customWidth="1"/>
     <col min="28" max="32" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" spans="1:32">
+    <row r="1" ht="16.5" spans="1:32">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -2618,7 +2618,7 @@
       </c>
       <c r="AF1" s="30"/>
     </row>
-    <row r="2" ht="16.2" spans="1:32">
+    <row r="2" ht="16.5" spans="1:32">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2691,7 +2691,7 @@
       <c r="AE2" s="14"/>
       <c r="AF2" s="14"/>
     </row>
-    <row r="3" ht="15.6" spans="2:32">
+    <row r="3" ht="16.5" spans="2:32">
       <c r="B3" s="7" t="s">
         <v>90</v>
       </c>
@@ -2729,7 +2729,7 @@
       <c r="AE3" s="10"/>
       <c r="AF3" s="10"/>
     </row>
-    <row r="4" ht="15.6" spans="1:32">
+    <row r="4" ht="16.5" spans="1:32">
       <c r="A4" s="11">
         <v>0</v>
       </c>
@@ -2777,7 +2777,7 @@
       <c r="AE4" s="33"/>
       <c r="AF4" s="33"/>
     </row>
-    <row r="5" ht="15.6" spans="1:32">
+    <row r="5" ht="16.5" spans="1:32">
       <c r="A5" s="11">
         <v>1</v>
       </c>
@@ -2849,7 +2849,7 @@
       <c r="AE5" s="33"/>
       <c r="AF5" s="33"/>
     </row>
-    <row r="6" ht="15.6" spans="1:32">
+    <row r="6" ht="16.5" spans="1:32">
       <c r="A6" s="11">
         <v>2</v>
       </c>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="AF6" s="33"/>
     </row>
-    <row r="7" ht="15.6" spans="1:32">
+    <row r="7" ht="16.5" spans="1:32">
       <c r="A7" s="11">
         <v>3</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" ht="15.6" spans="1:32">
+    <row r="8" ht="16.5" spans="1:32">
       <c r="A8" s="11">
         <v>4</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" ht="15.6" spans="1:32">
+    <row r="9" ht="16.5" spans="1:32">
       <c r="A9" s="11">
         <v>5</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" ht="15.6" spans="1:32">
+    <row r="10" ht="16.5" spans="1:32">
       <c r="A10" s="11">
         <v>6</v>
       </c>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="AF10" s="33"/>
     </row>
-    <row r="11" ht="15.6" spans="1:32">
+    <row r="11" ht="16.5" spans="1:32">
       <c r="A11" s="11">
         <v>7</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" ht="15.6" spans="1:32">
+    <row r="12" ht="16.5" spans="1:32">
       <c r="A12" s="11">
         <v>8</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" ht="15.6" spans="1:32">
+    <row r="13" ht="16.5" spans="1:32">
       <c r="A13" s="11">
         <v>9</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" ht="15.6" spans="1:32">
+    <row r="14" ht="16.5" spans="1:32">
       <c r="A14" s="11">
         <v>10</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" ht="15.6" spans="1:32">
+    <row r="15" ht="16.5" spans="1:32">
       <c r="A15" s="11">
         <v>11</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" ht="15.6" spans="1:32">
+    <row r="16" ht="16.5" spans="1:32">
       <c r="A16" s="11">
         <v>12</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" ht="15.6" spans="1:32">
+    <row r="17" ht="16.5" spans="1:32">
       <c r="A17" s="11">
         <v>13</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" ht="15.6" spans="1:32">
+    <row r="18" ht="16.5" spans="1:32">
       <c r="A18" s="11">
         <v>14</v>
       </c>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="AF18" s="33"/>
     </row>
-    <row r="19" ht="15.6" spans="1:32">
+    <row r="19" ht="16.5" spans="1:32">
       <c r="A19" s="11">
         <v>15</v>
       </c>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="AF19" s="33"/>
     </row>
-    <row r="20" ht="15.6" spans="1:32">
+    <row r="20" ht="16.5" spans="1:32">
       <c r="A20" s="11">
         <v>16</v>
       </c>
@@ -4093,7 +4093,7 @@
       <c r="AE20" s="36"/>
       <c r="AF20" s="33"/>
     </row>
-    <row r="21" ht="15.6" spans="1:32">
+    <row r="21" ht="16.5" spans="1:32">
       <c r="A21" s="11">
         <v>17</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="AE21" s="36"/>
       <c r="AF21" s="33"/>
     </row>
-    <row r="22" ht="15.6" spans="1:32">
+    <row r="22" ht="16.5" spans="1:32">
       <c r="A22" s="11">
         <v>18</v>
       </c>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="AF22" s="33"/>
     </row>
-    <row r="23" ht="15.6" spans="1:32">
+    <row r="23" ht="16.5" spans="1:32">
       <c r="A23" s="11">
         <v>19</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" ht="15.6" spans="1:32">
+    <row r="24" ht="16.5" spans="1:32">
       <c r="A24" s="11">
         <v>20</v>
       </c>
@@ -4421,7 +4421,7 @@
       <c r="AE24" s="36"/>
       <c r="AF24" s="33"/>
     </row>
-    <row r="25" ht="15.6" spans="1:32">
+    <row r="25" ht="16.5" spans="1:32">
       <c r="A25" s="11">
         <v>21</v>
       </c>
@@ -4495,7 +4495,7 @@
       <c r="AE25" s="36"/>
       <c r="AF25" s="33"/>
     </row>
-    <row r="26" ht="15.6" spans="1:32">
+    <row r="26" ht="16.5" spans="1:32">
       <c r="A26" s="11">
         <v>22</v>
       </c>
@@ -4573,7 +4573,7 @@
       <c r="AE26" s="36"/>
       <c r="AF26" s="37"/>
     </row>
-    <row r="27" ht="15.6" spans="1:32">
+    <row r="27" ht="16.5" spans="1:32">
       <c r="A27" s="11">
         <v>23</v>
       </c>
@@ -4649,7 +4649,7 @@
       <c r="AE27" s="36"/>
       <c r="AF27" s="37"/>
     </row>
-    <row r="28" ht="15.6" spans="1:32">
+    <row r="28" ht="16.5" spans="1:32">
       <c r="A28" s="11">
         <v>24</v>
       </c>
@@ -4725,7 +4725,7 @@
       <c r="AE28" s="36"/>
       <c r="AF28" s="37"/>
     </row>
-    <row r="29" ht="15.6" spans="1:32">
+    <row r="29" ht="16.5" spans="1:32">
       <c r="A29" s="11">
         <v>25</v>
       </c>
@@ -4797,7 +4797,7 @@
       <c r="AE29" s="36"/>
       <c r="AF29" s="37"/>
     </row>
-    <row r="30" ht="15.6" spans="1:32">
+    <row r="30" ht="16.5" spans="1:32">
       <c r="A30" s="11" t="s">
         <v>140</v>
       </c>
@@ -4843,7 +4843,7 @@
       <c r="AE30" s="36"/>
       <c r="AF30" s="37"/>
     </row>
-    <row r="31" ht="15.6" spans="1:32">
+    <row r="31" ht="16.5" spans="1:32">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -4877,7 +4877,7 @@
       <c r="AE31" s="15"/>
       <c r="AF31" s="38"/>
     </row>
-    <row r="32" ht="15.6" spans="1:32">
+    <row r="32" ht="16.5" spans="1:32">
       <c r="A32" s="14" t="s">
         <v>146</v>
       </c>
@@ -4923,7 +4923,7 @@
       <c r="AE32" s="15"/>
       <c r="AF32" s="38"/>
     </row>
-    <row r="33" ht="15.6" spans="1:31">
+    <row r="33" ht="16.5" spans="1:31">
       <c r="A33" s="14" t="s">
         <v>148</v>
       </c>
@@ -4968,7 +4968,7 @@
       <c r="AD33" s="15"/>
       <c r="AE33" s="15"/>
     </row>
-    <row r="34" ht="15.6" spans="1:31">
+    <row r="34" ht="16.5" spans="1:31">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -5001,7 +5001,7 @@
       <c r="AD34" s="15"/>
       <c r="AE34" s="15"/>
     </row>
-    <row r="35" ht="15.6" spans="1:31">
+    <row r="35" ht="16.5" spans="1:31">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -5034,7 +5034,7 @@
       <c r="AD35" s="15"/>
       <c r="AE35" s="15"/>
     </row>
-    <row r="36" ht="15.6" spans="1:31">
+    <row r="36" ht="16.5" spans="1:31">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -5067,7 +5067,7 @@
       <c r="AD36" s="15"/>
       <c r="AE36" s="15"/>
     </row>
-    <row r="37" ht="15.6" spans="1:31">
+    <row r="37" ht="16.5" spans="1:31">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -5100,7 +5100,7 @@
       <c r="AD37" s="15"/>
       <c r="AE37" s="15"/>
     </row>
-    <row r="38" ht="15.6" spans="7:31">
+    <row r="38" ht="16.5" spans="7:31">
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>

</xml_diff>